<commit_message>
Add cascade FE data function
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_sir_badcascade1.xlsx
+++ b/tests/frameworks/framework_sir_badcascade1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BDB533-E33D-4C2F-A3D3-038044F45C96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0D10DC-02C9-43B4-9867-6410A3B698CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="7" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,9 +1314,7 @@
         <v>59</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1336,9 +1334,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1358,9 +1354,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1380,9 +1374,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
+      <c r="H5" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1474,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,9 +1518,7 @@
         <v>59</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1546,9 +1536,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1566,9 +1554,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1584,9 +1570,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
@@ -1602,9 +1586,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1620,9 +1602,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1640,9 +1620,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1660,9 +1638,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
         <v>34</v>
       </c>
@@ -1681,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>